<commit_message>
added overall stats, lost creek
</commit_message>
<xml_diff>
--- a/Yearly Reports/2018/Lost Creek/Lost Creek Report.xlsx
+++ b/Yearly Reports/2018/Lost Creek/Lost Creek Report.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FitzFishing\Yearly Reports\2018\Lost Creek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEE8C33-F877-4765-9AE2-6EAEC3C863AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C2AB3-341F-44EB-8DEF-78CE968420D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8DE2BBAA-EA86-4618-A5D1-9D67D132A723}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{8DE2BBAA-EA86-4618-A5D1-9D67D132A723}"/>
   </bookViews>
   <sheets>
-    <sheet name="2018" sheetId="1" r:id="rId1"/>
+    <sheet name="2017" sheetId="2" r:id="rId1"/>
+    <sheet name="2018" sheetId="1" r:id="rId2"/>
+    <sheet name="Overall Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="23">
   <si>
     <t>Lake/Pond</t>
   </si>
@@ -89,12 +91,18 @@
   <si>
     <t>Percent Species Caught</t>
   </si>
+  <si>
+    <t>Fishing Report 2017 Lost Creek</t>
+  </si>
+  <si>
+    <t>1 Cutthroat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,8 +149,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +177,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,11 +209,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,14 +247,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -231,6 +281,2052 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> species caught</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Rainbow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cutthroat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spake</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tiger</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCA7-44AE-B35D-996EB6E1438D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="84"/>
+        <c:gapDepth val="53"/>
+        <c:shape val="box"/>
+        <c:axId val="2103499520"/>
+        <c:axId val="2098783376"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="2103499520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2098783376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2098783376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2103499520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PERCENT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SPECIES CAUGHT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$5:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Rainbow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cutthroat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spake</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tiger</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50.943396226415096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.39622641509434</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8867924528301887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7735849056603774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-071B-4AD4-835C-8718EA862B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="291">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:tint val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="0" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D91A12-0E10-4028-9A6E-A345B5B891C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EFCE92B-169E-4D40-BC60-646EEA520BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,11 +2625,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA41687D-1154-48E9-99F5-076BCC3AEC5F}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="27" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="17">
+        <f>SUM(C4)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="17">
+        <f>AVERAGE(C4)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <f>SUM(E4/C5*100)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E5:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323EE9B-AB86-4873-AC4E-09D7B8B4629E}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,20 +2774,20 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -624,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -638,8 +2853,14 @@
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="F5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -653,14 +2874,20 @@
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -674,17 +2901,21 @@
       <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>15</v>
+      <c r="F7" s="7">
+        <f>SUM(F4/$D$9*100)</f>
+        <v>51.923076923076927</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUM(G4/$D$9*100)</f>
+        <v>42.307692307692307</v>
+      </c>
+      <c r="H7" s="7">
+        <f>SUM(H4/$D$9*100)</f>
+        <v>1.9230769230769231</v>
+      </c>
+      <c r="I7" s="7">
+        <f>SUM(I4/$D$9*100)</f>
+        <v>3.8461538461538463</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -700,22 +2931,6 @@
       </c>
       <c r="E8" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F8">
-        <f>SUM(F4/$D$9*100)</f>
-        <v>51.923076923076927</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ref="G8:I8" si="0">SUM(G4/$D$9*100)</f>
-        <v>42.307692307692307</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>1.9230769230769231</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>3.8461538461538463</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -748,8 +2963,141 @@
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F732B40A-C676-4E35-BDB2-7C35D38C3BAA}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <f>SUM('2018'!F4)</f>
+        <v>27</v>
+      </c>
+      <c r="B3" s="7">
+        <f>SUM('2017'!E4+'2018'!G4)</f>
+        <v>23</v>
+      </c>
+      <c r="C3" s="7">
+        <f>SUM('2018'!H4)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <f>SUM('2018'!I4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <f>SUM(A3/$B$8*100)</f>
+        <v>50.943396226415096</v>
+      </c>
+      <c r="B6" s="7">
+        <f t="shared" ref="B6:D6" si="0">SUM(B3/$B$8*100)</f>
+        <v>43.39622641509434</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8867924528301887</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>3.7735849056603774</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8">
+        <f>SUM('2017'!C5+'2018'!D9)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8">
+        <f>SUM('2017'!C6+'2018'!D10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9">
+        <f>SUM(B8/B9)</f>
+        <v>8.8333333333333339</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated lost creek + rockport
</commit_message>
<xml_diff>
--- a/Yearly Reports/2018/Lost Creek/Lost Creek Report.xlsx
+++ b/Yearly Reports/2018/Lost Creek/Lost Creek Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FitzFishing\Yearly Reports\2018\Lost Creek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\Fishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C2AB3-341F-44EB-8DEF-78CE968420D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1401A92B-3E10-4B6D-AE54-20D438D724F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{8DE2BBAA-EA86-4618-A5D1-9D67D132A723}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Lake/Pond</t>
   </si>
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,15 +247,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,6 +254,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,10 +509,10 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Rainbow</c:v>
+                  <c:v>Cutthroat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cutthroat</c:v>
+                  <c:v>Rainbow</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Spake</c:v>
@@ -527,10 +530,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -850,6 +853,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-AA39-43D5-8BEA-FB9D868500B6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -893,6 +901,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AA39-43D5-8BEA-FB9D868500B6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -936,6 +949,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-AA39-43D5-8BEA-FB9D868500B6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -979,6 +997,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-AA39-43D5-8BEA-FB9D868500B6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -986,10 +1009,10 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Rainbow</c:v>
+                  <c:v>Cutthroat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cutthroat</c:v>
+                  <c:v>Rainbow</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Spake</c:v>
@@ -1004,13 +1027,13 @@
             <c:numRef>
               <c:f>'Overall Stats'!$A$6:$D$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50.943396226415096</c:v>
+                  <c:v>43.39622641509434</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.39622641509434</c:v>
+                  <c:v>50.943396226415096</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.8867924528301887</c:v>
@@ -2646,8 +2669,8 @@
         <v>21</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -2660,25 +2683,25 @@
       <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2699,22 +2722,22 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="14">
         <f>SUM(C4)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -2725,7 +2748,7 @@
       <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="14">
         <f>AVERAGE(C4)</f>
         <v>1</v>
       </c>
@@ -2748,7 +2771,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,10 +2781,10 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.5">
@@ -2774,20 +2797,20 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -2800,10 +2823,10 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>14</v>
@@ -2827,10 +2850,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="7">
+        <v>22</v>
+      </c>
+      <c r="G4" s="7">
         <v>27</v>
-      </c>
-      <c r="G4" s="7">
-        <v>22</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -2853,12 +2876,12 @@
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -2875,10 +2898,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>14</v>
@@ -2901,19 +2924,19 @@
       <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="19">
         <f>SUM(F4/$D$9*100)</f>
+        <v>42.307692307692307</v>
+      </c>
+      <c r="G7" s="19">
+        <f>SUM(G4/$D$9*100)</f>
         <v>51.923076923076927</v>
       </c>
-      <c r="G7" s="7">
-        <f>SUM(G4/$D$9*100)</f>
-        <v>42.307692307692307</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="H7" s="19">
         <f>SUM(H4/$D$9*100)</f>
         <v>1.9230769230769231</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="19">
         <f>SUM(I4/$D$9*100)</f>
         <v>3.8461538461538463</v>
       </c>
@@ -2974,31 +2997,30 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>14</v>
@@ -3009,12 +3031,12 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <f>SUM('2018'!F4)</f>
+        <f>SUM('2017'!E4+'2018'!F4)</f>
+        <v>23</v>
+      </c>
+      <c r="B3" s="7">
+        <f>SUM('2018'!G4)</f>
         <v>27</v>
-      </c>
-      <c r="B3" s="7">
-        <f>SUM('2017'!E4+'2018'!G4)</f>
-        <v>23</v>
       </c>
       <c r="C3" s="7">
         <f>SUM('2018'!H4)</f>
@@ -3026,19 +3048,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>14</v>
@@ -3048,19 +3070,19 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="19">
         <f>SUM(A3/$B$8*100)</f>
+        <v>43.39622641509434</v>
+      </c>
+      <c r="B6" s="19">
+        <f>SUM(B3/$B$8*100)</f>
         <v>50.943396226415096</v>
       </c>
-      <c r="B6" s="7">
-        <f t="shared" ref="B6:D6" si="0">SUM(B3/$B$8*100)</f>
-        <v>43.39622641509434</v>
-      </c>
-      <c r="C6" s="7">
-        <f t="shared" si="0"/>
+      <c r="C6" s="19">
+        <f t="shared" ref="B6:D6" si="0">SUM(C3/$B$8*100)</f>
         <v>1.8867924528301887</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="19">
         <f t="shared" si="0"/>
         <v>3.7735849056603774</v>
       </c>

</xml_diff>